<commit_message>
Updated w better actuator model
</commit_message>
<xml_diff>
--- a/Lab1/Lab1_Data.xlsx
+++ b/Lab1/Lab1_Data.xlsx
@@ -377,7 +377,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3096,11 +3095,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="405593760"/>
-        <c:axId val="405588272"/>
+        <c:axId val="393573440"/>
+        <c:axId val="393574224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="405593760"/>
+        <c:axId val="393573440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3143,7 +3142,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3203,12 +3201,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405588272"/>
+        <c:crossAx val="393574224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="405588272"/>
+        <c:axId val="393574224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,7 +3249,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3311,7 +3308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405593760"/>
+        <c:crossAx val="393573440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3910,11 +3907,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="405583568"/>
-        <c:axId val="405591016"/>
+        <c:axId val="393567560"/>
+        <c:axId val="393571480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="405583568"/>
+        <c:axId val="393567560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3971,12 +3968,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405591016"/>
+        <c:crossAx val="393571480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="405591016"/>
+        <c:axId val="393571480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4033,7 +4030,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405583568"/>
+        <c:crossAx val="393567560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4126,7 +4123,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5441,11 +5437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="405591408"/>
-        <c:axId val="405589056"/>
+        <c:axId val="393568344"/>
+        <c:axId val="393575008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="405591408"/>
+        <c:axId val="393568344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5488,7 +5484,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5548,12 +5543,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405589056"/>
+        <c:crossAx val="393575008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="405589056"/>
+        <c:axId val="393575008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5596,7 +5591,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5656,7 +5650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405591408"/>
+        <c:crossAx val="393568344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5874,11 +5868,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="405585920"/>
-        <c:axId val="405589448"/>
+        <c:axId val="393572264"/>
+        <c:axId val="393572656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="405585920"/>
+        <c:axId val="393572264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5935,12 +5929,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405589448"/>
+        <c:crossAx val="393572656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="405589448"/>
+        <c:axId val="393572656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5997,7 +5991,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405585920"/>
+        <c:crossAx val="393572264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6208,11 +6202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="405590232"/>
-        <c:axId val="405591800"/>
+        <c:axId val="393577752"/>
+        <c:axId val="393578144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="405590232"/>
+        <c:axId val="393577752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6269,12 +6263,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405591800"/>
+        <c:crossAx val="393578144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="405591800"/>
+        <c:axId val="393578144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6331,7 +6325,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405590232"/>
+        <c:crossAx val="393577752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6542,11 +6536,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="405592584"/>
-        <c:axId val="405589840"/>
+        <c:axId val="393580496"/>
+        <c:axId val="393580104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="405592584"/>
+        <c:axId val="393580496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6603,12 +6597,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405589840"/>
+        <c:crossAx val="393580104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="405589840"/>
+        <c:axId val="393580104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6665,7 +6659,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="405592584"/>
+        <c:crossAx val="393580496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6876,11 +6870,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="409660296"/>
-        <c:axId val="409656768"/>
+        <c:axId val="393579320"/>
+        <c:axId val="397546336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="409660296"/>
+        <c:axId val="393579320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6937,12 +6931,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409656768"/>
+        <c:crossAx val="397546336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="409656768"/>
+        <c:axId val="397546336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6999,7 +6993,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409660296"/>
+        <c:crossAx val="393579320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7309,11 +7303,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="409655200"/>
-        <c:axId val="409654416"/>
+        <c:axId val="397546728"/>
+        <c:axId val="397547120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="409655200"/>
+        <c:axId val="397546728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7370,12 +7364,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409654416"/>
+        <c:crossAx val="397547120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="409654416"/>
+        <c:axId val="397547120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7432,7 +7426,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409655200"/>
+        <c:crossAx val="397546728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7669,11 +7663,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="409659904"/>
-        <c:axId val="409652848"/>
+        <c:axId val="397547512"/>
+        <c:axId val="397553784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="409659904"/>
+        <c:axId val="397547512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7730,12 +7724,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409652848"/>
+        <c:crossAx val="397553784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="409652848"/>
+        <c:axId val="397553784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7792,7 +7786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409659904"/>
+        <c:crossAx val="397547512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12791,7 +12785,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B979B6D7-32D6-4E62-A756-39D08B9CADBE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B979B6D7-32D6-4E62-A756-39D08B9CADBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12834,7 +12828,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B877E292-546B-4A63-A8E4-E4CD866FD40A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B877E292-546B-4A63-A8E4-E4CD866FD40A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12870,7 +12864,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB849EB3-FF48-43D3-B43B-142602FB0CE8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB849EB3-FF48-43D3-B43B-142602FB0CE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12911,7 +12905,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7114E12C-B8B3-4B60-A110-6766F09E714A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7114E12C-B8B3-4B60-A110-6766F09E714A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12949,7 +12943,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{663B122D-C18C-466F-A386-F55FB188238D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{663B122D-C18C-466F-A386-F55FB188238D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12987,7 +12981,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FCE9C7D0-76D3-48A9-BDD6-7A7A74FB45B0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCE9C7D0-76D3-48A9-BDD6-7A7A74FB45B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13025,7 +13019,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{85EADD52-5041-4CC1-87C6-66C10226B1DD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85EADD52-5041-4CC1-87C6-66C10226B1DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13063,7 +13057,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEAFD47A-E80A-4C81-A70A-E0AFF2A5E3C1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEAFD47A-E80A-4C81-A70A-E0AFF2A5E3C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13101,7 +13095,7 @@
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EB834279-E02D-4F14-A524-49E3AAEDDA55}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB834279-E02D-4F14-A524-49E3AAEDDA55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>